<commit_message>
add traductor and fix audios
</commit_message>
<xml_diff>
--- a/src/assets/excel/multicuentas.xlsx
+++ b/src/assets/excel/multicuentas.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -420,47 +420,39 @@
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v>Angel</v>
+        <v>XDIABLA01</v>
       </c>
       <c r="B3" t="str">
-        <v>xTokio, TH, LifeToxic, NotLife, Arima, TG, Joker, TG, xJokerx, TH, TG, Anteiku, Kaneki, TG</v>
+        <v>Cubita01, xDIABLAx, XIBANDIDAIX, JuanEscutia, XCLEOPATRA1X, II, Loba, Cubita1, minidiabla, lobiore, foodbabe, Maiky150701, minibandida, DIABLILLABB</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="str">
-        <v>XDIABLA01</v>
+        <v>Ashb0rn</v>
       </c>
       <c r="B4" t="str">
-        <v>Cubita01, xDIABLAx, XIBANDIDAIX, JuanEscutia, XCLEOPATRA1X, II, Loba, Cubita1, minidiabla, lobiore, foodbabe, Maiky150701, minibandida, DIABLILLABB</v>
+        <v>Ashb0rn</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="str">
-        <v>Ashb0rn</v>
+        <v>David</v>
       </c>
       <c r="B5" t="str">
-        <v>Ashb0rn</v>
+        <v>Ghostk47, CandyCandy69, yoshitecojo, candystore69</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="str">
-        <v>David</v>
+        <v>Angel</v>
       </c>
       <c r="B6" t="str">
-        <v>Ghostk47, CandyCandy69, yoshitecojo, candystore69</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="str">
-        <v>julian</v>
-      </c>
-      <c r="B7" t="str">
-        <v>cuenta 1, cuwenta 2, cue ta3</v>
+        <v>xTokio TH, LifeToxic, NotLife, Joker TG, xJokerx TH, TG anteiku, Kaneki TG, Arima TG</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:B7"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:B6"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
add traductor and avisos
</commit_message>
<xml_diff>
--- a/src/assets/excel/multicuentas.xlsx
+++ b/src/assets/excel/multicuentas.xlsx
@@ -1,41 +1,82 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
   <workbookPr codeName="ThisWorkbook"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\Node\Bot-TH-Wsp\src\assets\excel\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02FC0978-1FBD-4D20-A70E-4E897DBDF28B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
     <sheet name="Multicuentas" sheetId="1" r:id="rId1"/>
   </sheets>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
-<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
-  <metadataTypes count="1">
-    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
-  </metadataTypes>
-  <futureMetadata name="XLDAPR" count="1">
-    <bk>
-      <extLst>
-        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
-          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
-        </ext>
-      </extLst>
-    </bk>
-  </futureMetadata>
-  <cellMetadata count="1">
-    <bk>
-      <rc t="1" v="0"/>
-    </bk>
-  </cellMetadata>
-</metadata>
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
+  <si>
+    <t>Nombre</t>
+  </si>
+  <si>
+    <t>Cuentas</t>
+  </si>
+  <si>
+    <t>Axel</t>
+  </si>
+  <si>
+    <t>XDIABLA01</t>
+  </si>
+  <si>
+    <t>Ashb0rn</t>
+  </si>
+  <si>
+    <t>David</t>
+  </si>
+  <si>
+    <t>Ghostk47, CandyCandy69, yoshitecojo, candystore69</t>
+  </si>
+  <si>
+    <t>Angel</t>
+  </si>
+  <si>
+    <t>xTokio TH, LifeToxic, NotLife, Joker TG, xJokerx TH, TG anteiku, Kaneki TG, Arima TG</t>
+  </si>
+  <si>
+    <t>SoNy5, Nyd4n, thslayer, Foodmil, Craksoder25, Megaman6</t>
+  </si>
+  <si>
+    <t>Cubita01, xDIABLAx, XIBANDIDAIX, JuanEscutia, XCLEOPATRA1X, II Loba, Cubita1, minidiabla, lobiore, foodbabe, Maiky150701, minibandida, DIABLILLABB, Maiky140701</t>
+  </si>
+  <si>
+    <t>Brandon</t>
+  </si>
+  <si>
+    <t>Brandon 22, Deshuesado</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:vt="http://schemas.openxmlformats.org/officeDocument/2006/docPropsVTypes">
-  <numFmts count="1">
-    <numFmt numFmtId="56" formatCode="&quot;上午/下午 &quot;hh&quot;時&quot;mm&quot;分&quot;ss&quot;秒 &quot;"/>
-  </numFmts>
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -65,13 +106,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -396,63 +445,78 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6:XFD6"/>
+    </sheetView>
   </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="128.875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1">
-      <c r="A1" t="str">
-        <v>Nombre</v>
-      </c>
-      <c r="B1" t="str">
-        <v>Cuentas</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="str">
-        <v>Axel</v>
-      </c>
-      <c r="B2" t="str">
-        <v>SoNy5, Nyd4n, thslayer, Foodmil, Craksoder25</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="str">
-        <v>XDIABLA01</v>
-      </c>
-      <c r="B3" t="str">
-        <v>Cubita01, xDIABLAx, XIBANDIDAIX, JuanEscutia, XCLEOPATRA1X, II, Loba, Cubita1, minidiabla, lobiore, foodbabe, Maiky150701, minibandida, DIABLILLABB</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="str">
-        <v>Ashb0rn</v>
-      </c>
-      <c r="B4" t="str">
-        <v>Ashb0rn</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="str">
-        <v>David</v>
-      </c>
-      <c r="B5" t="str">
-        <v>Ghostk47, CandyCandy69, yoshitecojo, candystore69</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="str">
-        <v>Angel</v>
-      </c>
-      <c r="B6" t="str">
-        <v>xTokio TH, LifeToxic, NotLife, Joker TG, xJokerx TH, TG anteiku, Kaneki TG, Arima TG</v>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:B6"/>
+    <ignoredError sqref="A1:B1 A4:B6 A2 A3" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>